<commit_message>
change in config file
</commit_message>
<xml_diff>
--- a/data/credits.xlsx
+++ b/data/credits.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -424,67 +424,27 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>ACC-1756806307308</v>
+        <v>ACC-1756905141601</v>
       </c>
       <c r="B2" t="str">
-        <v>a.arslan@agilemitservices.ae</v>
+        <v>ali.arslan@agiemtech.ae</v>
       </c>
       <c r="C2">
         <v>500</v>
       </c>
       <c r="D2">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F2" t="str">
-        <v>Active</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>ACC-1756807317744</v>
-      </c>
-      <c r="B3" t="str">
-        <v>rpa@agilemitservices.ae</v>
-      </c>
-      <c r="C3">
-        <v>500</v>
-      </c>
-      <c r="D3">
-        <v>500</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3" t="str">
-        <v>Active</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>ACC-1756807892091</v>
-      </c>
-      <c r="B4" t="str">
-        <v>aqsa.ayub@agilemtech.ae</v>
-      </c>
-      <c r="C4">
-        <v>500</v>
-      </c>
-      <c r="D4">
-        <v>100</v>
-      </c>
-      <c r="E4">
-        <v>400</v>
-      </c>
-      <c r="F4" t="str">
         <v>Active</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>